<commit_message>
Small update to the readme file and example data
</commit_message>
<xml_diff>
--- a/inst/extdata/example_data/with_unstained/220309-FlowCore-SymphonyA3-CD4.xlsx
+++ b/inst/extdata/example_data/with_unstained/220309-FlowCore-SymphonyA3-CD4.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>CODE</t>
   </si>
   <si>
-    <t>Pos plaat</t>
-  </si>
-  <si>
     <t>Antibody name</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>F0014</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>CD4</t>
   </si>
   <si>
@@ -68,22 +62,10 @@
     <t>SK3</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
     <t>F0021</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>BV-421</t>
-  </si>
-  <si>
-    <t>C9</t>
   </si>
   <si>
     <t>F0031</t>
@@ -210,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -236,19 +218,6 @@
     <border>
       <left/>
       <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFB7B7B7"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFB7B7B7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
         <color rgb="FFB7B7B7"/>
       </right>
       <top style="medium">
@@ -265,17 +234,6 @@
       </left>
       <right style="medium">
         <color rgb="FFB7B7B7"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFB7B7B7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -307,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -315,25 +273,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -616,243 +568,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="10" max="10" width="19.5234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:11" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>355</v>
+      </c>
+      <c r="E2" s="5">
+        <v>395</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5">
+        <v>405</v>
+      </c>
+      <c r="E3" s="5">
+        <v>421</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5">
+        <v>488</v>
+      </c>
+      <c r="E4" s="5">
+        <v>520</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>578</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5">
+        <v>633</v>
+      </c>
+      <c r="E6" s="5">
+        <v>719</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
         <v>38</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7">
-        <v>355</v>
-      </c>
-      <c r="F2" s="7">
-        <v>395</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7">
-        <v>405</v>
-      </c>
-      <c r="F3" s="7">
-        <v>421</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="7">
-        <v>488</v>
-      </c>
-      <c r="F4" s="7">
-        <v>520</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="7">
-        <v>578</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="7">
-        <v>633</v>
-      </c>
-      <c r="F6" s="7">
-        <v>719</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>